<commit_message>
added generation cost to output excel
</commit_message>
<xml_diff>
--- a/CASURECO II/Historical_CASURECO_II_GC_Breakdown.xlsx
+++ b/CASURECO II/Historical_CASURECO_II_GC_Breakdown.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,10 +452,15 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Generation Charge</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Power Supplier ID</t>
         </is>
@@ -479,10 +484,15 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>2 .7423</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>Jun-2024</t>
         </is>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>1</v>
       </c>
     </row>
@@ -504,10 +514,15 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
+          <t>2 .7423</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>Jun-2024</t>
         </is>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>2</v>
       </c>
     </row>
@@ -529,10 +544,15 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
+          <t>2 .7423</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
           <t>Jun-2024</t>
         </is>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>3</v>
       </c>
     </row>
@@ -550,10 +570,15 @@
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
+          <t>2 .7423</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
           <t>Jun-2024</t>
         </is>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>4</v>
       </c>
     </row>
@@ -575,10 +600,15 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
+          <t>6 .7472</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
           <t>May-2024</t>
         </is>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>5</v>
       </c>
     </row>
@@ -600,10 +630,15 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
+          <t>6 .7472</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
           <t>May-2024</t>
         </is>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -625,10 +660,15 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
+          <t>6 .7472</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
           <t>May-2024</t>
         </is>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
         <v>2</v>
       </c>
     </row>
@@ -650,10 +690,15 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
+          <t>6 .7472</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
           <t>May-2024</t>
         </is>
       </c>
-      <c r="E9" t="n">
+      <c r="F9" t="n">
         <v>3</v>
       </c>
     </row>
@@ -671,10 +716,15 @@
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr">
         <is>
+          <t>6 .7472</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
           <t>May-2024</t>
         </is>
       </c>
-      <c r="E10" t="n">
+      <c r="F10" t="n">
         <v>4</v>
       </c>
     </row>
@@ -696,10 +746,15 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
+          <t>4 .9881</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
           <t>Apr-2024</t>
         </is>
       </c>
-      <c r="E11" t="n">
+      <c r="F11" t="n">
         <v>5</v>
       </c>
     </row>
@@ -721,10 +776,15 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
+          <t>4 .9881</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
           <t>Apr-2024</t>
         </is>
       </c>
-      <c r="E12" t="n">
+      <c r="F12" t="n">
         <v>1</v>
       </c>
     </row>
@@ -746,10 +806,15 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
+          <t>4 .9881</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
           <t>Apr-2024</t>
         </is>
       </c>
-      <c r="E13" t="n">
+      <c r="F13" t="n">
         <v>2</v>
       </c>
     </row>
@@ -771,10 +836,15 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
+          <t>4 .9881</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
           <t>Apr-2024</t>
         </is>
       </c>
-      <c r="E14" t="n">
+      <c r="F14" t="n">
         <v>3</v>
       </c>
     </row>
@@ -792,10 +862,15 @@
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr">
         <is>
+          <t>4 .9881</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
           <t>Apr-2024</t>
         </is>
       </c>
-      <c r="E15" t="n">
+      <c r="F15" t="n">
         <v>4</v>
       </c>
     </row>
@@ -817,10 +892,15 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
+          <t>7 .9383</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
           <t>Jul-2024</t>
         </is>
       </c>
-      <c r="E16" t="n">
+      <c r="F16" t="n">
         <v>1</v>
       </c>
     </row>
@@ -842,10 +922,15 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
+          <t>7 .9383</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
           <t>Jul-2024</t>
         </is>
       </c>
-      <c r="E17" t="n">
+      <c r="F17" t="n">
         <v>2</v>
       </c>
     </row>
@@ -867,10 +952,15 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
+          <t>7 .9383</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
           <t>Jul-2024</t>
         </is>
       </c>
-      <c r="E18" t="n">
+      <c r="F18" t="n">
         <v>3</v>
       </c>
     </row>
@@ -888,10 +978,15 @@
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr">
         <is>
+          <t>7 .9383</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
           <t>Jul-2024</t>
         </is>
       </c>
-      <c r="E19" t="n">
+      <c r="F19" t="n">
         <v>4</v>
       </c>
     </row>

</xml_diff>